<commit_message>
Working on exergy destruction calcluations.
</commit_message>
<xml_diff>
--- a/data/HeatLossFlows.xlsx
+++ b/data/HeatLossFlows.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB65F93-8015-6E4A-AC44-E30C798B6942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA31A1C-B6B1-AF48-B490-72CD9A920507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23060" yWindow="4340" windowWidth="28040" windowHeight="17440" xr2:uid="{742590E8-047E-1447-91ED-17B8D0993C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>Industry</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>**** Need to decide a temperature</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>TemperatureK</t>
   </si>
 </sst>
 </file>
@@ -266,11 +272,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -607,19 +612,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1AC2A6-D39E-A444-B5A1-5D796C28F5AC}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,355 +633,627 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1144</v>
+      </c>
+      <c r="D2">
+        <f>1 - 298.15/C2</f>
+        <v>0.73937937062937065</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <f>600+273.15</f>
+        <v>873.15</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D35" si="0">1 - 298.15/C3</f>
+        <v>0.65853518868464755</v>
+      </c>
+      <c r="E3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <f>500+273.15</f>
+        <v>773.15</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.61436978594063252</v>
+      </c>
+      <c r="E4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <f>2500+273.15</f>
+        <v>2773.15</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6">
+        <v>1573</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.81045772409408778</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <f>25+273.15</f>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8">
+        <f>(1200-32)*5/9 + 273.15</f>
+        <v>922.03888888888889</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.67664053697421778</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <f>200+273.15</f>
+        <v>473.15</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.36986156609954557</v>
+      </c>
+      <c r="E9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" ref="C9:C29" si="1">25+273.15</f>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16">
+        <f>2500+273.15</f>
+        <v>2773.15</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18">
+        <f>2500+273.15</f>
+        <v>2773.15</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19">
+        <f>2500+273.15</f>
+        <v>2773.15</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21">
+        <f t="shared" ref="C21:C29" si="2">2500+273.15</f>
+        <v>2773.15</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>2773.15</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.8924868831473235</v>
+      </c>
+      <c r="E29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1173</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0.74582267689684567</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31">
+        <v>1573</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0.81045772409408778</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" ref="C32:C34" si="3">25+273.15</f>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33">
+        <v>2373</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0.87435735356089339</v>
+      </c>
+      <c r="E33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="3"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35">
+        <v>1144</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>0.73937937062937065</v>
+      </c>
+      <c r="E35" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{C8BF8FD3-09EB-A24C-96AE-02A6FAC1C1FB}"/>
-    <hyperlink ref="C31" r:id="rId2" xr:uid="{235A2FDB-7FDE-2447-A2D4-4CD848ECE1AB}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{2018C0C2-0D95-AA4A-81A8-86F9B4FF2499}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{C8BF8FD3-09EB-A24C-96AE-02A6FAC1C1FB}"/>
+    <hyperlink ref="E31" r:id="rId2" xr:uid="{235A2FDB-7FDE-2447-A2D4-4CD848ECE1AB}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{2018C0C2-0D95-AA4A-81A8-86F9B4FF2499}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Remove calculation of balances. No longer needed.
</commit_message>
<xml_diff>
--- a/data/HeatLossFlows.xlsx
+++ b/data/HeatLossFlows.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA31A1C-B6B1-AF48-B490-72CD9A920507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C13A21F-7860-5149-9A91-E9BADD1325E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23060" yWindow="4340" windowWidth="28040" windowHeight="17440" xr2:uid="{742590E8-047E-1447-91ED-17B8D0993C1D}"/>
   </bookViews>
@@ -615,7 +615,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,7 +800,7 @@
         <v>47</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C9:C29" si="1">25+273.15</f>
+        <f t="shared" ref="C10:C20" si="1">25+273.15</f>
         <v>298.14999999999998</v>
       </c>
       <c r="D10">

</xml_diff>